<commit_message>
Achievement system and bugs fixed
</commit_message>
<xml_diff>
--- a/Assets/Resources/Localization.xlsx
+++ b/Assets/Resources/Localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elegetic\TellltheAuthority\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAE48A7-6D9C-4203-AAD9-37B549926E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4B1341-360F-443C-B2D3-C5BE9CB0F66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="1390" windowWidth="19200" windowHeight="11170" xr2:uid="{C21F6677-7B9D-48C9-8722-1AB02A4EB084}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{C21F6677-7B9D-48C9-8722-1AB02A4EB084}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="170">
   <si>
     <t>EN_GB</t>
   </si>
@@ -464,16 +464,106 @@
   </si>
   <si>
     <t>当前总分：</t>
+  </si>
+  <si>
+    <t>ACHIEVEMENTS</t>
+  </si>
+  <si>
+    <t>成就</t>
+  </si>
+  <si>
+    <t>PERFECT CITY</t>
+  </si>
+  <si>
+    <t>PERFECT RAINFOREST</t>
+  </si>
+  <si>
+    <t>PERFECT HARBOUR</t>
+  </si>
+  <si>
+    <t>PERFECT TOWN</t>
+  </si>
+  <si>
+    <t>PERFECT COUNTRYSIDE</t>
+  </si>
+  <si>
+    <t>完美城市</t>
+  </si>
+  <si>
+    <t>完美雨林</t>
+  </si>
+  <si>
+    <t>完美港湾</t>
+  </si>
+  <si>
+    <t>完美小镇</t>
+  </si>
+  <si>
+    <t>完美郊外</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL PERFECT! </t>
+  </si>
+  <si>
+    <t>皆传！</t>
+  </si>
+  <si>
+    <t>GET ALL REPORTS CORRECT IN LEVEL 1</t>
+  </si>
+  <si>
+    <t>第一关所有举报正确</t>
+  </si>
+  <si>
+    <t>GET ALL REPORTS CORRECT IN LEVEL 2</t>
+  </si>
+  <si>
+    <t>第二关所有举报正确</t>
+  </si>
+  <si>
+    <t>GET ALL REPORTS CORRECT IN LEVEL 3</t>
+  </si>
+  <si>
+    <t>GET ALL REPORTS CORRECT IN LEVEL 4</t>
+  </si>
+  <si>
+    <t>GET ALL REPORTS CORRECT IN LEVEL 5</t>
+  </si>
+  <si>
+    <t>第三关所有举报正确</t>
+  </si>
+  <si>
+    <t>第四关所有举报正确</t>
+  </si>
+  <si>
+    <t>第五关所有举报正确</t>
+  </si>
+  <si>
+    <t>GET ALL REPORTS CORRECT IN THE GAME</t>
+  </si>
+  <si>
+    <t>游戏中所有举报皆正确</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>？？？</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -841,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679472E8-4440-48DF-8D5D-1D03DFA57972}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1462,7 +1552,128 @@
         <v>129</v>
       </c>
     </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>